<commit_message>
Change model Qwen3B - HF
</commit_message>
<xml_diff>
--- a/data/output/table_writer_test.xlsx
+++ b/data/output/table_writer_test.xlsx
@@ -444,7 +444,7 @@
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="27" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
-    <col width="13" customWidth="1" min="12" max="12"/>
+    <col width="11" customWidth="1" min="12" max="12"/>
     <col width="22" customWidth="1" min="13" max="13"/>
     <col width="26" customWidth="1" min="14" max="14"/>
     <col width="13" customWidth="1" min="15" max="15"/>
@@ -548,28 +548,12 @@
           <t>ул. Тестовая, 1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ЗУ: -</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>74:36:0000000:123 ()</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>1000 м²</t>
@@ -577,27 +561,15 @@
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>ООО Ромашка</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Автоматически</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>Иванов И.И.</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>до</t>
-        </is>
-      </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
           <t>test.pdf</t>

</xml_diff>